<commit_message>
Añadiendo imagen del pseudocódigo al archivo
</commit_message>
<xml_diff>
--- a/Ejemplo Insertion Sort.xlsx
+++ b/Ejemplo Insertion Sort.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alvaro\Desktop\ÁLVARO\TERCER_CURSO_2\COCO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alvaro\Desktop\ÁLVARO\TERCER_CURSO_2\COCO\Ejemplo_Insertion_Sort\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F34CE7AC-490A-4C43-B514-D515C791128F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{879960B0-2F07-452D-A386-BEA4E3800F83}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C24A8A8E-76E4-4F88-948C-DC2D29AC39FC}"/>
   </bookViews>
@@ -225,6 +225,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>9949</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A13CF51A-70E7-4BD4-9A3E-A70A948500E4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="762000" y="2495551"/>
+          <a:ext cx="5334000" cy="3248448"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -527,7 +576,7 @@
   <dimension ref="B3:N38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1119,5 +1168,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>